<commit_message>
table added to the pip network analysis
</commit_message>
<xml_diff>
--- a/python/pipe_network_analysis/data/2x2/diameter.xlsx
+++ b/python/pipe_network_analysis/data/2x2/diameter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian\Documents\work\engineering_solutions\python\pipe_network_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian\Documents\work\engineering_solutions\python\pipe_network_analysis\data\2x2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539A2342-0FD2-415B-BCD9-5BDEFB481FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A8E276-6810-4B58-A0B0-885626D89D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -413,65 +413,40 @@
       <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
-      </c>
-      <c r="E3">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>0.2</v>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
-      </c>
-      <c r="G5">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>0.15</v>
+        <v>0.9</v>
+      </c>
+      <c r="D5">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>